<commit_message>
<made some changes on the dataset.xlsx>
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmet/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmet/Desktop/GitHub Folder/excel-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC526C20-6D89-064D-8416-9008D783D954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52290A0F-4F15-2242-A6DB-61659F0489F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="680" windowWidth="28040" windowHeight="17420" xr2:uid="{BE92B275-1F41-DD48-B1AF-C4F9E03510FE}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,7 +576,7 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>